<commit_message>
Updated instructor in project proposal and updated project's gantt chart colors
</commit_message>
<xml_diff>
--- a/papers/skyline-crs-project-gantt-chart.xlsx
+++ b/papers/skyline-crs-project-gantt-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDF\DevOps\skyline-crs\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32AF865-D94F-4826-A07C-C47D83237070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF5A53D-F06A-4891-9114-60B9930C434F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>טבלת ניהול משאבים - Skyline CRS</t>
   </si>
@@ -296,7 +296,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,14 +334,16 @@
       </patternFill>
     </fill>
     <fill>
-      <gradientFill degree="45">
-        <stop position="0">
-          <color theme="4" tint="0.59999389629810485"/>
-        </stop>
-        <stop position="1">
-          <color theme="9" tint="0.59999389629810485"/>
-        </stop>
-      </gradientFill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -430,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -469,7 +471,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -478,58 +524,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -811,13 +816,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK32"/>
+  <dimension ref="A1:AK33"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -829,336 +834,336 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:37" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="S2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="U2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="V2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="W2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="17" t="s">
+      <c r="X2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="Y2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="Z2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AA2" s="17" t="s">
+      <c r="AA2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="17" t="s">
+      <c r="AB2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AC2" s="17" t="s">
+      <c r="AC2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="AD2" s="17" t="s">
+      <c r="AD2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AE2" s="17" t="s">
+      <c r="AE2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AF2" s="17" t="s">
+      <c r="AF2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AG2" s="17" t="s">
+      <c r="AG2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="AH2" s="17" t="s">
+      <c r="AH2" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="AI2" s="17" t="s">
+      <c r="AI2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AJ2" s="17" t="s">
+      <c r="AJ2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AK2" s="17" t="s">
+      <c r="AK2" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:37" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19">
+      <c r="A3" s="34"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="15">
         <v>44475</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="15">
         <v>44482</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="15">
         <v>44489</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="15">
         <v>44496</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="15">
         <v>44503</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="15">
         <v>44510</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="15">
         <v>44517</v>
       </c>
-      <c r="K3" s="19">
+      <c r="K3" s="15">
         <v>44524</v>
       </c>
-      <c r="L3" s="19">
+      <c r="L3" s="15">
         <v>44531</v>
       </c>
-      <c r="M3" s="19">
+      <c r="M3" s="15">
         <v>44538</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="15">
         <v>44545</v>
       </c>
-      <c r="O3" s="19">
+      <c r="O3" s="15">
         <v>44552</v>
       </c>
-      <c r="P3" s="19">
+      <c r="P3" s="15">
         <v>44559</v>
       </c>
-      <c r="Q3" s="19">
+      <c r="Q3" s="15">
         <v>44566</v>
       </c>
-      <c r="R3" s="19">
+      <c r="R3" s="15">
         <v>44573</v>
       </c>
-      <c r="S3" s="19">
+      <c r="S3" s="15">
         <v>44580</v>
       </c>
-      <c r="T3" s="19">
+      <c r="T3" s="15">
         <v>44587</v>
       </c>
-      <c r="U3" s="19">
+      <c r="U3" s="15">
         <v>44594</v>
       </c>
-      <c r="V3" s="19">
+      <c r="V3" s="15">
         <v>44601</v>
       </c>
-      <c r="W3" s="19">
+      <c r="W3" s="15">
         <v>44608</v>
       </c>
-      <c r="X3" s="19">
+      <c r="X3" s="15">
         <v>44615</v>
       </c>
-      <c r="Y3" s="19">
+      <c r="Y3" s="15">
         <v>44622</v>
       </c>
-      <c r="Z3" s="19">
+      <c r="Z3" s="15">
         <v>44629</v>
       </c>
-      <c r="AA3" s="19">
+      <c r="AA3" s="15">
         <v>44636</v>
       </c>
-      <c r="AB3" s="19">
+      <c r="AB3" s="15">
         <v>44643</v>
       </c>
-      <c r="AC3" s="19">
+      <c r="AC3" s="15">
         <v>44650</v>
       </c>
-      <c r="AD3" s="19">
+      <c r="AD3" s="15">
         <v>44657</v>
       </c>
-      <c r="AE3" s="19">
+      <c r="AE3" s="15">
         <v>44664</v>
       </c>
-      <c r="AF3" s="19">
+      <c r="AF3" s="15">
         <v>44671</v>
       </c>
-      <c r="AG3" s="19">
+      <c r="AG3" s="15">
         <v>44678</v>
       </c>
-      <c r="AH3" s="19">
+      <c r="AH3" s="15">
         <v>44685</v>
       </c>
-      <c r="AI3" s="19">
+      <c r="AI3" s="15">
         <v>44692</v>
       </c>
-      <c r="AJ3" s="19">
+      <c r="AJ3" s="15">
         <v>44699</v>
       </c>
-      <c r="AK3" s="19">
+      <c r="AK3" s="15">
         <v>44706</v>
       </c>
     </row>
     <row r="4" spans="1:37" s="7" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="20">
+      <c r="A4" s="34"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="16">
         <v>44481</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="16">
         <v>44488</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="16">
         <v>44495</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="16">
         <v>44502</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="16">
         <v>44509</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="16">
         <v>44516</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="16">
         <v>44523</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="16">
         <v>44530</v>
       </c>
-      <c r="L4" s="20">
+      <c r="L4" s="16">
         <v>44537</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="16">
         <v>44544</v>
       </c>
-      <c r="N4" s="20">
+      <c r="N4" s="16">
         <v>44551</v>
       </c>
-      <c r="O4" s="20">
+      <c r="O4" s="16">
         <v>44558</v>
       </c>
-      <c r="P4" s="20">
+      <c r="P4" s="16">
         <v>44565</v>
       </c>
-      <c r="Q4" s="20">
+      <c r="Q4" s="16">
         <v>44572</v>
       </c>
-      <c r="R4" s="20">
+      <c r="R4" s="16">
         <v>44579</v>
       </c>
-      <c r="S4" s="20">
+      <c r="S4" s="16">
         <v>44586</v>
       </c>
-      <c r="T4" s="20">
+      <c r="T4" s="16">
         <v>44593</v>
       </c>
-      <c r="U4" s="20">
+      <c r="U4" s="16">
         <v>44600</v>
       </c>
-      <c r="V4" s="20">
+      <c r="V4" s="16">
         <v>44607</v>
       </c>
-      <c r="W4" s="20">
+      <c r="W4" s="16">
         <v>44614</v>
       </c>
-      <c r="X4" s="20">
+      <c r="X4" s="16">
         <v>44621</v>
       </c>
-      <c r="Y4" s="20">
+      <c r="Y4" s="16">
         <v>44628</v>
       </c>
-      <c r="Z4" s="20">
+      <c r="Z4" s="16">
         <v>44635</v>
       </c>
-      <c r="AA4" s="20">
+      <c r="AA4" s="16">
         <v>44642</v>
       </c>
-      <c r="AB4" s="20">
+      <c r="AB4" s="16">
         <v>44649</v>
       </c>
-      <c r="AC4" s="20">
+      <c r="AC4" s="16">
         <v>44656</v>
       </c>
-      <c r="AD4" s="20">
+      <c r="AD4" s="16">
         <v>44663</v>
       </c>
-      <c r="AE4" s="20">
+      <c r="AE4" s="16">
         <v>44670</v>
       </c>
-      <c r="AF4" s="20">
+      <c r="AF4" s="16">
         <v>44677</v>
       </c>
-      <c r="AG4" s="20">
+      <c r="AG4" s="16">
         <v>44684</v>
       </c>
-      <c r="AH4" s="20">
+      <c r="AH4" s="16">
         <v>44691</v>
       </c>
-      <c r="AI4" s="20">
+      <c r="AI4" s="16">
         <v>44698</v>
       </c>
-      <c r="AJ4" s="20">
+      <c r="AJ4" s="16">
         <v>44705</v>
       </c>
-      <c r="AK4" s="20">
+      <c r="AK4" s="16">
         <v>44712</v>
       </c>
     </row>
@@ -1172,15 +1177,15 @@
       <c r="C5" s="11">
         <v>3</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="29"/>
+      <c r="L5" s="25"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
@@ -1220,12 +1225,12 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="30"/>
+      <c r="L6" s="26"/>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
@@ -1266,11 +1271,11 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
-      <c r="L7" s="30"/>
+      <c r="L7" s="26"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
@@ -1312,10 +1317,10 @@
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="24"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="11"/>
-      <c r="L8" s="30"/>
+      <c r="L8" s="26"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
@@ -1358,9 +1363,9 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="30"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="26"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
@@ -1405,8 +1410,8 @@
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="28"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
@@ -1450,10 +1455,10 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="L11" s="30"/>
+      <c r="L11" s="26"/>
       <c r="M11" s="11"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
@@ -1495,11 +1500,11 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
-      <c r="L12" s="30"/>
+      <c r="L12" s="26"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
-      <c r="P12" s="31"/>
+      <c r="P12" s="35"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
@@ -1540,14 +1545,14 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
-      <c r="L13" s="30"/>
+      <c r="L13" s="26"/>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
       <c r="T13" s="11"/>
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
@@ -1585,7 +1590,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
-      <c r="L14" s="30"/>
+      <c r="L14" s="26"/>
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
@@ -1593,7 +1598,7 @@
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
-      <c r="T14" s="31"/>
+      <c r="T14" s="35"/>
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
@@ -1630,7 +1635,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
-      <c r="L15" s="30"/>
+      <c r="L15" s="26"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
@@ -1639,9 +1644,9 @@
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="22"/>
+      <c r="W15" s="22"/>
       <c r="X15" s="11"/>
       <c r="Y15" s="11"/>
       <c r="Z15" s="11"/>
@@ -1675,7 +1680,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="30"/>
+      <c r="L16" s="26"/>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
@@ -1687,9 +1692,9 @@
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
       <c r="AA16" s="11"/>
       <c r="AB16" s="11"/>
       <c r="AC16" s="11"/>
@@ -1720,7 +1725,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
-      <c r="L17" s="30"/>
+      <c r="L17" s="26"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
@@ -1735,7 +1740,7 @@
       <c r="X17" s="11"/>
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
-      <c r="AA17" s="26"/>
+      <c r="AA17" s="22"/>
       <c r="AB17" s="11"/>
       <c r="AC17" s="11"/>
       <c r="AD17" s="11"/>
@@ -1765,7 +1770,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
-      <c r="L18" s="30"/>
+      <c r="L18" s="26"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
@@ -1781,8 +1786,8 @@
       <c r="Y18" s="11"/>
       <c r="Z18" s="11"/>
       <c r="AA18" s="11"/>
-      <c r="AB18" s="26"/>
-      <c r="AC18" s="25"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="21"/>
       <c r="AD18" s="11"/>
       <c r="AE18" s="11"/>
       <c r="AF18" s="11"/>
@@ -1810,7 +1815,7 @@
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
-      <c r="L19" s="30"/>
+      <c r="L19" s="26"/>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
@@ -1827,8 +1832,8 @@
       <c r="Z19" s="11"/>
       <c r="AA19" s="11"/>
       <c r="AB19" s="11"/>
-      <c r="AC19" s="26"/>
-      <c r="AD19" s="25"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="21"/>
       <c r="AE19" s="11"/>
       <c r="AF19" s="11"/>
       <c r="AG19" s="11"/>
@@ -1855,7 +1860,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
-      <c r="L20" s="30"/>
+      <c r="L20" s="26"/>
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
@@ -1873,10 +1878,10 @@
       <c r="AA20" s="11"/>
       <c r="AB20" s="11"/>
       <c r="AC20" s="11"/>
-      <c r="AD20" s="26"/>
-      <c r="AE20" s="26"/>
-      <c r="AF20" s="26"/>
-      <c r="AG20" s="25"/>
+      <c r="AD20" s="22"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="22"/>
+      <c r="AG20" s="21"/>
       <c r="AH20" s="11"/>
       <c r="AI20" s="11"/>
       <c r="AJ20" s="11"/>
@@ -1900,7 +1905,7 @@
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="32"/>
+      <c r="L21" s="27"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
@@ -1921,7 +1926,7 @@
       <c r="AD21" s="10"/>
       <c r="AE21" s="10"/>
       <c r="AF21" s="10"/>
-      <c r="AG21" s="33"/>
+      <c r="AG21" s="28"/>
       <c r="AH21" s="10"/>
       <c r="AI21" s="10"/>
       <c r="AJ21" s="10"/>
@@ -1945,7 +1950,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
-      <c r="L22" s="30"/>
+      <c r="L22" s="26"/>
       <c r="M22" s="11"/>
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
@@ -1967,10 +1972,10 @@
       <c r="AE22" s="11"/>
       <c r="AF22" s="11"/>
       <c r="AG22" s="11"/>
-      <c r="AH22" s="23"/>
-      <c r="AI22" s="23"/>
-      <c r="AJ22" s="23"/>
-      <c r="AK22" s="23"/>
+      <c r="AH22" s="19"/>
+      <c r="AI22" s="19"/>
+      <c r="AJ22" s="19"/>
+      <c r="AK22" s="19"/>
     </row>
     <row r="23" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
@@ -1980,7 +1985,7 @@
       <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="29"/>
     </row>
     <row r="26" spans="1:37" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
@@ -1991,37 +1996,43 @@
       </c>
     </row>
     <row r="27" spans="1:37" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:37" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="24"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:37" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:37" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:37" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="30"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26"/>
+      <c r="B32" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="4"/>
+    <row r="33" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>